<commit_message>
Actualizacion a archivo de riesgos y tiempos
</commit_message>
<xml_diff>
--- a/Seguimiento/Soporte-riesgos/SeguimientoActualizaciónTiemposGithub.xlsx
+++ b/Seguimiento/Soporte-riesgos/SeguimientoActualizaciónTiemposGithub.xlsx
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Ciclo2 Semana 1</t>
   </si>
@@ -994,7 +994,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1087,9 @@
       <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1154,7 +1156,9 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>

</xml_diff>